<commit_message>
Added Rolling forecast contable
</commit_message>
<xml_diff>
--- a/data/Template.xlsx
+++ b/data/Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ibtest2020.sharepoint.com/sites/ia.ibtest/Documentos compartidos/02. Projects/Rolling Forecast - Finance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/c_angel/Documents/python/forecast_app_v3/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{C6CEB4B1-45EF-9B4B-9397-091DD13372DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24334C97-5343-0049-A9CB-F3414E56907B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CDABD1-E675-9C45-A12B-9FDC5AD42B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="620" windowWidth="38400" windowHeight="19780" xr2:uid="{FE7EDCC4-FC9C-1048-9C72-413AFED1C9D3}"/>
+    <workbookView xWindow="36000" yWindow="620" windowWidth="38400" windowHeight="19780" xr2:uid="{FE7EDCC4-FC9C-1048-9C72-413AFED1C9D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -68,31 +68,31 @@
     <t>Costo de venta por Backlog PM</t>
   </si>
   <si>
-    <t>Facturacion por Forecast &lt; 60%</t>
-  </si>
-  <si>
     <t>BU</t>
   </si>
   <si>
     <t>TODAS</t>
   </si>
   <si>
-    <t>Costo de venta por Forecast &lt; 60%</t>
-  </si>
-  <si>
-    <t>Facturacion por Forecast&lt; 60%</t>
-  </si>
-  <si>
-    <t>Facturacion por Forecast &gt;= 60%</t>
-  </si>
-  <si>
-    <t>Costo de venta por Forecast &gt;= 60%</t>
-  </si>
-  <si>
     <t>…</t>
   </si>
   <si>
     <t>REP, SWD, TRN</t>
+  </si>
+  <si>
+    <t>Facturacion por Pipeline &gt;= 60%</t>
+  </si>
+  <si>
+    <t>Facturacion por Pipeline&lt; 60%</t>
+  </si>
+  <si>
+    <t>Facturacion por Pipeline &lt; 60%</t>
+  </si>
+  <si>
+    <t>Costo de venta por Pipeline &gt;= 60%</t>
+  </si>
+  <si>
+    <t>Costo de venta por Pipeline &lt; 60%</t>
   </si>
 </sst>
 </file>
@@ -496,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D71550A-3A52-FF4B-9E51-3B97DD6ADA00}">
   <dimension ref="A1:AB85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G75" sqref="G75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,7 +517,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="3">
         <v>45962</v>
@@ -553,7 +553,7 @@
         <v>46266</v>
       </c>
       <c r="O1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
@@ -564,7 +564,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -586,7 +586,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -608,7 +608,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -630,7 +630,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -646,13 +646,13 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -668,13 +668,13 @@
     </row>
     <row r="7" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -690,13 +690,13 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -712,13 +712,13 @@
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -734,13 +734,13 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -756,13 +756,13 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -778,13 +778,13 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -800,13 +800,13 @@
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -958,7 +958,7 @@
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>7</v>
@@ -991,7 +991,7 @@
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>8</v>
@@ -1024,7 +1024,7 @@
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>7</v>
@@ -1058,7 +1058,7 @@
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>8</v>
@@ -1092,7 +1092,7 @@
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>7</v>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>8</v>
@@ -1159,7 +1159,7 @@
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>7</v>
@@ -1192,7 +1192,7 @@
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>8</v>
@@ -1302,7 +1302,7 @@
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>7</v>
@@ -1324,7 +1324,7 @@
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>8</v>
@@ -1346,7 +1346,7 @@
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>7</v>
@@ -1368,7 +1368,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>8</v>
@@ -1390,7 +1390,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>7</v>
@@ -1412,7 +1412,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>8</v>
@@ -1434,7 +1434,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>7</v>
@@ -1456,7 +1456,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>8</v>
@@ -1566,7 +1566,7 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>7</v>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>8</v>
@@ -1610,7 +1610,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>7</v>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>8</v>
@@ -1654,7 +1654,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>7</v>
@@ -1676,7 +1676,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>8</v>
@@ -1698,7 +1698,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>7</v>
@@ -1720,7 +1720,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>8</v>
@@ -1830,7 +1830,7 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>7</v>
@@ -1852,7 +1852,7 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>8</v>
@@ -1874,7 +1874,7 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>7</v>
@@ -1896,7 +1896,7 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>8</v>
@@ -1918,7 +1918,7 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>7</v>
@@ -1940,7 +1940,7 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>8</v>
@@ -1962,7 +1962,7 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>7</v>
@@ -1984,7 +1984,7 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>8</v>
@@ -2012,7 +2012,7 @@
         <v>7</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
@@ -2034,7 +2034,7 @@
         <v>8</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
@@ -2056,7 +2056,7 @@
         <v>7</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
@@ -2078,7 +2078,7 @@
         <v>8</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
@@ -2094,13 +2094,13 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
@@ -2116,13 +2116,13 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
@@ -2138,13 +2138,13 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
@@ -2160,13 +2160,13 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
@@ -2182,13 +2182,13 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
@@ -2226,13 +2226,13 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
@@ -2248,13 +2248,13 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
@@ -2467,6 +2467,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="caf8a2a9-d283-4d69-a44f-bf13743108e6" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="459acbf3-697c-4cdc-89a6-8a33fc3c21e6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010073F3A862BA1ADC4F9DDDC4D751DD301B" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="1e813ef934c78d2c6e0f1a278dfc7693">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="459acbf3-697c-4cdc-89a6-8a33fc3c21e6" xmlns:ns3="caf8a2a9-d283-4d69-a44f-bf13743108e6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="be61f5629c75c3696be7900f790f6786" ns2:_="" ns3:_="">
     <xsd:import namespace="459acbf3-697c-4cdc-89a6-8a33fc3c21e6"/>
@@ -2667,41 +2687,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="caf8a2a9-d283-4d69-a44f-bf13743108e6" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="459acbf3-697c-4cdc-89a6-8a33fc3c21e6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3B759F4-C9CB-487A-AACD-2AF853EBA6C0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44E5BD90-5B1F-4C6B-9B1B-8B0491856D99}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="459acbf3-697c-4cdc-89a6-8a33fc3c21e6"/>
-    <ds:schemaRef ds:uri="caf8a2a9-d283-4d69-a44f-bf13743108e6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2724,9 +2713,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44E5BD90-5B1F-4C6B-9B1B-8B0491856D99}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3B759F4-C9CB-487A-AACD-2AF853EBA6C0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="459acbf3-697c-4cdc-89a6-8a33fc3c21e6"/>
+    <ds:schemaRef ds:uri="caf8a2a9-d283-4d69-a44f-bf13743108e6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>